<commit_message>
added two key graphs
</commit_message>
<xml_diff>
--- a/Hoboken_weekday.xlsx
+++ b/Hoboken_weekday.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
   <si>
     <t>6:44AM</t>
   </si>
@@ -348,9 +348,6 @@
     <t>11:19PM</t>
   </si>
   <si>
-    <t>11:39PM</t>
-  </si>
-  <si>
     <t>PATH_arrival_Hoboken_weekday</t>
   </si>
   <si>
@@ -520,9 +517,6 @@
   </si>
   <si>
     <t>11:37 PM </t>
-  </si>
-  <si>
-    <t>12:07 AM </t>
   </si>
   <si>
     <t>lightrail_departure_Hoboken_weekday</t>
@@ -921,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -935,10 +929,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -946,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -954,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -962,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -970,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -978,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -986,7 +980,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -994,7 +988,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1002,7 +996,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1010,7 +1004,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1018,7 +1012,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1026,7 +1020,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1034,7 +1028,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1042,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1050,7 +1044,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1058,7 +1052,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1066,7 +1060,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1074,7 +1068,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1082,7 +1076,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1090,7 +1084,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1098,7 +1092,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1106,7 +1100,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1114,7 +1108,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1122,7 +1116,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1130,7 +1124,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1138,7 +1132,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1146,7 +1140,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1154,7 +1148,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1162,7 +1156,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1170,7 +1164,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1178,7 +1172,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1186,7 +1180,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1194,7 +1188,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1202,7 +1196,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1210,7 +1204,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1218,7 +1212,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1226,7 +1220,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1234,7 +1228,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1242,7 +1236,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1250,7 +1244,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1258,7 +1252,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1266,7 +1260,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1274,7 +1268,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1282,7 +1276,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1290,7 +1284,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1298,7 +1292,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1306,7 +1300,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1314,7 +1308,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1322,7 +1316,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1330,7 +1324,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1338,7 +1332,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1346,7 +1340,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1354,7 +1348,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1362,7 +1356,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1370,7 +1364,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1378,7 +1372,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1386,16 +1380,14 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="B58" s="1"/>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
@@ -1655,11 +1647,6 @@
     <row r="110" spans="1:1">
       <c r="A110" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>